<commit_message>
remaining issues for #114
</commit_message>
<xml_diff>
--- a/sample_apps/simple_ja/simple-scenario-ja.xlsx
+++ b/sample_apps/simple_ja/simple-scenario-ja.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nakano\system\dialbb\dialbb-next\sample_apps\simple_ja\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE480DAC-3FC8-470E-8FDB-F31027F90E45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1250AA38-7B72-464F-8985-3464DB676615}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C3566FB2-A815-41D8-9347-99D11DD601B4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C3566FB2-A815-41D8-9347-99D11DD601B4}"/>
   </bookViews>
   <sheets>
     <sheet name="scenario" sheetId="1" r:id="rId1"/>
@@ -238,27 +238,7 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>申し訳ありません。内部エラーがおきてしまいました。今日はありがとうございました。</t>
-    <rPh sb="0" eb="1">
-      <t>モウ</t>
-    </rPh>
-    <rPh sb="2" eb="3">
-      <t>ワケ</t>
-    </rPh>
-    <rPh sb="9" eb="11">
-      <t>ナイブ</t>
-    </rPh>
-    <rPh sb="25" eb="27">
-      <t>キョウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Y</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>わかりました。今日はお時間ありがとうございました。</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -340,10 +320,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>{location}ですね。今日はお時間ありがとうございました。</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>ラーメンの地方を言う</t>
     <rPh sb="5" eb="7">
       <t>チホウ</t>
@@ -394,6 +370,15 @@
   </si>
   <si>
     <t>_set(&amp;location, #地方)</t>
+  </si>
+  <si>
+    <t>{location}ですね。今日はお時間ありがとうございました。(clear_chat_window:yes)</t>
+  </si>
+  <si>
+    <t>わかりました。今日はお時間ありがとうございました。(clear_chat_window:yes)</t>
+  </si>
+  <si>
+    <t>申し訳ありません。内部エラーがおきてしまいました。今日はありがとうございました。(clear_chat_window:yes)</t>
   </si>
 </sst>
 </file>
@@ -849,8 +834,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC9D1DC6-E066-4D71-9ECD-01107058A46B}">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:H16"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
@@ -871,7 +856,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>0</v>
@@ -894,17 +879,17 @@
     </row>
     <row r="2" spans="1:8" s="3" customFormat="1">
       <c r="A2" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
       <c r="F2" s="9"/>
       <c r="G2" s="9" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="H2" s="9" t="s">
         <v>17</v>
@@ -912,13 +897,13 @@
     </row>
     <row r="3" spans="1:8" s="4" customFormat="1" ht="45">
       <c r="A3" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>17</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>9</v>
@@ -934,7 +919,7 @@
     </row>
     <row r="4" spans="1:8" s="4" customFormat="1" ht="30">
       <c r="A4" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>17</v>
@@ -954,7 +939,7 @@
     </row>
     <row r="5" spans="1:8" s="4" customFormat="1">
       <c r="A5" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B5" s="10" t="s">
         <v>17</v>
@@ -974,7 +959,7 @@
     </row>
     <row r="6" spans="1:8" s="4" customFormat="1">
       <c r="A6" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>17</v>
@@ -990,7 +975,7 @@
     </row>
     <row r="7" spans="1:8" s="1" customFormat="1" ht="30">
       <c r="A7" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>2</v>
@@ -1012,7 +997,7 @@
     </row>
     <row r="8" spans="1:8" s="1" customFormat="1">
       <c r="A8" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>2</v>
@@ -1032,7 +1017,7 @@
     </row>
     <row r="9" spans="1:8" s="1" customFormat="1">
       <c r="A9" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>2</v>
@@ -1052,7 +1037,7 @@
     </row>
     <row r="10" spans="1:8" s="1" customFormat="1" ht="30">
       <c r="A10" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>2</v>
@@ -1072,14 +1057,14 @@
     </row>
     <row r="11" spans="1:8" s="1" customFormat="1">
       <c r="A11" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>2</v>
       </c>
       <c r="C11" s="8"/>
       <c r="D11" s="8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
@@ -1090,7 +1075,7 @@
     </row>
     <row r="12" spans="1:8" s="5" customFormat="1" ht="45">
       <c r="A12" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B12" s="11" t="s">
         <v>3</v>
@@ -1110,7 +1095,7 @@
     </row>
     <row r="13" spans="1:8" s="6" customFormat="1" ht="60">
       <c r="A13" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B13" s="12" t="s">
         <v>21</v>
@@ -1125,10 +1110,10 @@
         <v>26</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="H13" s="12" t="s">
         <v>16</v>
@@ -1136,7 +1121,7 @@
     </row>
     <row r="14" spans="1:8" s="6" customFormat="1" ht="45">
       <c r="A14" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B14" s="12" t="s">
         <v>21</v>
@@ -1149,10 +1134,10 @@
         <v>26</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G14" s="12" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="H14" s="12" t="s">
         <v>26</v>
@@ -1160,7 +1145,7 @@
     </row>
     <row r="15" spans="1:8" s="6" customFormat="1" ht="30">
       <c r="A15" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B15" s="12" t="s">
         <v>21</v>
@@ -1171,25 +1156,25 @@
         <v>26</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="H15" s="12" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:8" s="6" customFormat="1" ht="45">
       <c r="A16" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B16" s="12" t="s">
         <v>21</v>
       </c>
       <c r="C16" s="12"/>
       <c r="D16" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E16" s="12"/>
       <c r="F16" s="12"/>
@@ -1200,7 +1185,7 @@
     </row>
     <row r="17" spans="1:8" s="3" customFormat="1" ht="45">
       <c r="A17" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B17" s="9" t="s">
         <v>23</v>
@@ -1220,13 +1205,13 @@
     </row>
     <row r="18" spans="1:8" s="4" customFormat="1" ht="45">
       <c r="A18" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B18" s="10" t="s">
         <v>16</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
@@ -1238,13 +1223,13 @@
     </row>
     <row r="19" spans="1:8" s="4" customFormat="1" ht="30">
       <c r="A19" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B19" s="10" t="s">
         <v>26</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D19" s="10"/>
       <c r="E19" s="10"/>
@@ -1256,34 +1241,34 @@
     </row>
     <row r="20" spans="1:8" s="1" customFormat="1" ht="45">
       <c r="A20" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D20" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E20" s="8" t="s">
         <v>41</v>
-      </c>
-      <c r="E20" s="8" t="s">
-        <v>44</v>
       </c>
       <c r="F20" s="8"/>
       <c r="G20" s="8" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="H20" s="8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:8" s="1" customFormat="1" ht="30">
       <c r="A21" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
@@ -1296,13 +1281,13 @@
     </row>
     <row r="22" spans="1:8" s="6" customFormat="1" ht="45">
       <c r="A22" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="D22" s="12"/>
       <c r="E22" s="12"/>
@@ -1312,13 +1297,13 @@
     </row>
     <row r="23" spans="1:8" s="7" customFormat="1" ht="45">
       <c r="A23" s="13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B23" s="13" t="s">
         <v>18</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>33</v>
+        <v>52</v>
       </c>
       <c r="D23" s="13"/>
       <c r="E23" s="13"/>
@@ -1326,15 +1311,15 @@
       <c r="G23" s="13"/>
       <c r="H23" s="13"/>
     </row>
-    <row r="24" spans="1:8" s="4" customFormat="1" ht="60">
+    <row r="24" spans="1:8" s="4" customFormat="1" ht="75">
       <c r="A24" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B24" s="10" t="s">
         <v>30</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>31</v>
+        <v>53</v>
       </c>
       <c r="D24" s="10"/>
       <c r="E24" s="10"/>

</xml_diff>

<commit_message>
Bug in extracting aux_data fixed
</commit_message>
<xml_diff>
--- a/sample_apps/simple_ja/simple-scenario-ja.xlsx
+++ b/sample_apps/simple_ja/simple-scenario-ja.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nakano\system\dialbb\dialbb-next\sample_apps\simple_ja\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1250AA38-7B72-464F-8985-3464DB676615}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B967574B-4A85-4DB6-B8FC-4CC73D180CF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C3566FB2-A815-41D8-9347-99D11DD601B4}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{C3566FB2-A815-41D8-9347-99D11DD601B4}"/>
   </bookViews>
   <sheets>
     <sheet name="scenario" sheetId="1" r:id="rId1"/>
@@ -334,51 +334,38 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
+    <t>decide_greeting(&amp;greeting)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>_eq(#好きなラーメン, "豚骨ラーメン")</t>
+  </si>
+  <si>
+    <t>_set(&amp;topic_ramen, #好きなラーメン)</t>
+  </si>
+  <si>
+    <t>is_known_ramen(#好きなラーメン)</t>
+  </si>
+  <si>
+    <t>_set(&amp;topic_ramen, #好きなラーメン); get_ramen_location(*topic_ramen, &amp;location)</t>
+  </si>
+  <si>
+    <t>is_novel_ramen(#好きなラーメン)</t>
+  </si>
+  <si>
+    <t>_set(&amp;location, #地方)</t>
+  </si>
+  <si>
+    <t>{location}ですね。今日はお時間ありがとうございました。(clear_chat_window:yes)</t>
+  </si>
+  <si>
+    <t>わかりました。今日はお時間ありがとうございました。(clear_chat_window:yes)</t>
+  </si>
+  <si>
+    <t>申し訳ありません。内部エラーがおきてしまいました。今日はありがとうございました。(clear_chat_window:yes)</t>
+  </si>
+  <si>
     <t>{greeting}。今日はラーメンについて教えて下さい。ラーメンはよく食べますか？</t>
-    <rPh sb="11" eb="13">
-      <t>キョウ</t>
-    </rPh>
-    <rPh sb="22" eb="23">
-      <t>オシ</t>
-    </rPh>
-    <rPh sb="25" eb="26">
-      <t>クダ</t>
-    </rPh>
-    <rPh sb="36" eb="37">
-      <t>タ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>decide_greeting(&amp;greeting)</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>_eq(#好きなラーメン, "豚骨ラーメン")</t>
-  </si>
-  <si>
-    <t>_set(&amp;topic_ramen, #好きなラーメン)</t>
-  </si>
-  <si>
-    <t>is_known_ramen(#好きなラーメン)</t>
-  </si>
-  <si>
-    <t>_set(&amp;topic_ramen, #好きなラーメン); get_ramen_location(*topic_ramen, &amp;location)</t>
-  </si>
-  <si>
-    <t>is_novel_ramen(#好きなラーメン)</t>
-  </si>
-  <si>
-    <t>_set(&amp;location, #地方)</t>
-  </si>
-  <si>
-    <t>{location}ですね。今日はお時間ありがとうございました。(clear_chat_window:yes)</t>
-  </si>
-  <si>
-    <t>わかりました。今日はお時間ありがとうございました。(clear_chat_window:yes)</t>
-  </si>
-  <si>
-    <t>申し訳ありません。内部エラーがおきてしまいました。今日はありがとうございました。(clear_chat_window:yes)</t>
   </si>
 </sst>
 </file>
@@ -834,24 +821,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC9D1DC6-E066-4D71-9ECD-01107058A46B}">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="8.5703125" style="2"/>
-    <col min="2" max="2" width="19.42578125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="29.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.28515625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="33.42578125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="8.59765625" style="2"/>
+    <col min="2" max="2" width="19.3984375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="29.59765625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.86328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.265625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="33.3984375" style="2" customWidth="1"/>
     <col min="7" max="7" width="39" style="2" customWidth="1"/>
-    <col min="8" max="8" width="20.5703125" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="8.5703125" style="2"/>
+    <col min="8" max="8" width="20.59765625" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="8.59765625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="30">
+    <row r="1" spans="1:8" s="1" customFormat="1">
       <c r="A1" s="8" t="s">
         <v>6</v>
       </c>
@@ -889,13 +876,13 @@
       <c r="E2" s="9"/>
       <c r="F2" s="9"/>
       <c r="G2" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H2" s="9" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="4" customFormat="1" ht="45">
+    <row r="3" spans="1:8" s="4" customFormat="1" ht="42.75">
       <c r="A3" s="10" t="s">
         <v>31</v>
       </c>
@@ -903,7 +890,7 @@
         <v>17</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>9</v>
@@ -917,7 +904,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="4" customFormat="1" ht="30">
+    <row r="4" spans="1:8" s="4" customFormat="1">
       <c r="A4" s="10" t="s">
         <v>31</v>
       </c>
@@ -973,7 +960,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="1" customFormat="1" ht="30">
+    <row r="7" spans="1:8" s="1" customFormat="1">
       <c r="A7" s="8" t="s">
         <v>31</v>
       </c>
@@ -1035,7 +1022,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="1" customFormat="1" ht="30">
+    <row r="10" spans="1:8" s="1" customFormat="1">
       <c r="A10" s="8" t="s">
         <v>31</v>
       </c>
@@ -1073,7 +1060,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="5" customFormat="1" ht="45">
+    <row r="12" spans="1:8" s="5" customFormat="1" ht="28.5">
       <c r="A12" s="11" t="s">
         <v>31</v>
       </c>
@@ -1093,7 +1080,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="6" customFormat="1" ht="60">
+    <row r="13" spans="1:8" s="6" customFormat="1" ht="57">
       <c r="A13" s="12" t="s">
         <v>31</v>
       </c>
@@ -1110,16 +1097,16 @@
         <v>26</v>
       </c>
       <c r="F13" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="G13" s="12" t="s">
         <v>45</v>
-      </c>
-      <c r="G13" s="12" t="s">
-        <v>46</v>
       </c>
       <c r="H13" s="12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:8" s="6" customFormat="1" ht="45">
+    <row r="14" spans="1:8" s="6" customFormat="1" ht="28.5">
       <c r="A14" s="12" t="s">
         <v>31</v>
       </c>
@@ -1134,16 +1121,16 @@
         <v>26</v>
       </c>
       <c r="F14" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="G14" s="12" t="s">
         <v>47</v>
-      </c>
-      <c r="G14" s="12" t="s">
-        <v>48</v>
       </c>
       <c r="H14" s="12" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:8" s="6" customFormat="1" ht="30">
+    <row r="15" spans="1:8" s="6" customFormat="1" ht="28.5">
       <c r="A15" s="12" t="s">
         <v>31</v>
       </c>
@@ -1156,16 +1143,16 @@
         <v>26</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H15" s="12" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:8" s="6" customFormat="1" ht="45">
+    <row r="16" spans="1:8" s="6" customFormat="1" ht="28.5">
       <c r="A16" s="12" t="s">
         <v>31</v>
       </c>
@@ -1183,7 +1170,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:8" s="3" customFormat="1" ht="45">
+    <row r="17" spans="1:8" s="3" customFormat="1" ht="28.5">
       <c r="A17" s="9" t="s">
         <v>31</v>
       </c>
@@ -1203,7 +1190,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:8" s="4" customFormat="1" ht="45">
+    <row r="18" spans="1:8" s="4" customFormat="1" ht="42.75">
       <c r="A18" s="10" t="s">
         <v>31</v>
       </c>
@@ -1221,7 +1208,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:8" s="4" customFormat="1" ht="30">
+    <row r="19" spans="1:8" s="4" customFormat="1" ht="28.5">
       <c r="A19" s="10" t="s">
         <v>31</v>
       </c>
@@ -1239,7 +1226,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:8" s="1" customFormat="1" ht="45">
+    <row r="20" spans="1:8" s="1" customFormat="1" ht="42.75">
       <c r="A20" s="8" t="s">
         <v>31</v>
       </c>
@@ -1257,13 +1244,13 @@
       </c>
       <c r="F20" s="8"/>
       <c r="G20" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H20" s="8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:8" s="1" customFormat="1" ht="30">
+    <row r="21" spans="1:8" s="1" customFormat="1" ht="28.5">
       <c r="A21" s="8" t="s">
         <v>31</v>
       </c>
@@ -1279,7 +1266,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:8" s="6" customFormat="1" ht="45">
+    <row r="22" spans="1:8" s="6" customFormat="1" ht="42.75">
       <c r="A22" s="12" t="s">
         <v>31</v>
       </c>
@@ -1287,7 +1274,7 @@
         <v>40</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D22" s="12"/>
       <c r="E22" s="12"/>
@@ -1295,7 +1282,7 @@
       <c r="G22" s="12"/>
       <c r="H22" s="12"/>
     </row>
-    <row r="23" spans="1:8" s="7" customFormat="1" ht="45">
+    <row r="23" spans="1:8" s="7" customFormat="1" ht="42.75">
       <c r="A23" s="13" t="s">
         <v>31</v>
       </c>
@@ -1303,7 +1290,7 @@
         <v>18</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D23" s="13"/>
       <c r="E23" s="13"/>
@@ -1311,7 +1298,7 @@
       <c r="G23" s="13"/>
       <c r="H23" s="13"/>
     </row>
-    <row r="24" spans="1:8" s="4" customFormat="1" ht="75">
+    <row r="24" spans="1:8" s="4" customFormat="1" ht="57">
       <c r="A24" s="10" t="s">
         <v>31</v>
       </c>
@@ -1319,7 +1306,7 @@
         <v>30</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D24" s="10"/>
       <c r="E24" s="10"/>

</xml_diff>

<commit_message>
simple ja scenario reverted
</commit_message>
<xml_diff>
--- a/sample_apps/simple_ja/simple-scenario-ja.xlsx
+++ b/sample_apps/simple_ja/simple-scenario-ja.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nakano\system\dialbb\dialbb-next\sample_apps\simple_ja\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B967574B-4A85-4DB6-B8FC-4CC73D180CF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8821F9D8-C6FC-4012-B6DC-7ED8645F63D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{C3566FB2-A815-41D8-9347-99D11DD601B4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C3566FB2-A815-41D8-9347-99D11DD601B4}"/>
   </bookViews>
   <sheets>
     <sheet name="scenario" sheetId="1" r:id="rId1"/>
@@ -85,13 +85,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>ラーメンお好きなんですね。</t>
-    <rPh sb="5" eb="6">
-      <t>ス</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>そうですね。</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -365,7 +358,10 @@
     <t>申し訳ありません。内部エラーがおきてしまいました。今日はありがとうございました。(clear_chat_window:yes)</t>
   </si>
   <si>
-    <t>{greeting}。今日はラーメンについて教えて下さい。ラーメンはよく食べますか？</t>
+    <t xml:space="preserve">{greeting}。今日はラーメンについて教えて下さい。ラーメンはよく食べますか？ </t>
+  </si>
+  <si>
+    <t>ラーメンお好きなんですね。</t>
   </si>
 </sst>
 </file>
@@ -822,7 +818,7 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="14.25"/>
@@ -843,7 +839,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>0</v>
@@ -858,7 +854,7 @@
         <v>4</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H1" s="8" t="s">
         <v>1</v>
@@ -866,31 +862,31 @@
     </row>
     <row r="2" spans="1:8" s="3" customFormat="1">
       <c r="A2" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
       <c r="F2" s="9"/>
       <c r="G2" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="4" customFormat="1" ht="42.75">
       <c r="A3" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>9</v>
@@ -906,14 +902,14 @@
     </row>
     <row r="4" spans="1:8" s="4" customFormat="1">
       <c r="A4" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E4" s="10" t="s">
         <v>3</v>
@@ -926,17 +922,17 @@
     </row>
     <row r="5" spans="1:8" s="4" customFormat="1">
       <c r="A5" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C5" s="10"/>
       <c r="D5" s="10" t="s">
         <v>5</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
@@ -946,10 +942,10 @@
     </row>
     <row r="6" spans="1:8" s="4" customFormat="1">
       <c r="A6" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C6" s="10"/>
       <c r="D6" s="10"/>
@@ -957,305 +953,305 @@
       <c r="F6" s="10"/>
       <c r="G6" s="10"/>
       <c r="H6" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="1" customFormat="1">
       <c r="A7" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>2</v>
       </c>
       <c r="C7" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="8" t="s">
-        <v>11</v>
-      </c>
       <c r="E7" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F7" s="8"/>
       <c r="G7" s="8"/>
       <c r="H7" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="1" customFormat="1">
       <c r="A8" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>2</v>
       </c>
       <c r="C8" s="8"/>
       <c r="D8" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
       <c r="H8" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:8" s="1" customFormat="1">
       <c r="A9" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>2</v>
       </c>
       <c r="C9" s="8"/>
       <c r="D9" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F9" s="8"/>
       <c r="G9" s="8"/>
       <c r="H9" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:8" s="1" customFormat="1">
       <c r="A10" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>2</v>
       </c>
       <c r="C10" s="8"/>
       <c r="D10" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F10" s="8"/>
       <c r="G10" s="8"/>
       <c r="H10" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:8" s="1" customFormat="1">
       <c r="A11" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>2</v>
       </c>
       <c r="C11" s="8"/>
       <c r="D11" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
       <c r="G11" s="8"/>
       <c r="H11" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:8" s="5" customFormat="1" ht="28.5">
       <c r="A12" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B12" s="11" t="s">
         <v>3</v>
       </c>
       <c r="C12" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="11" t="s">
         <v>19</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>20</v>
       </c>
       <c r="E12" s="11"/>
       <c r="F12" s="11"/>
       <c r="G12" s="11"/>
       <c r="H12" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:8" s="6" customFormat="1" ht="57">
       <c r="A13" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F13" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="G13" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="G13" s="12" t="s">
-        <v>45</v>
-      </c>
       <c r="H13" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:8" s="6" customFormat="1" ht="28.5">
       <c r="A14" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C14" s="12"/>
       <c r="D14" s="12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F14" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="G14" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="G14" s="12" t="s">
-        <v>47</v>
-      </c>
       <c r="H14" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:8" s="6" customFormat="1" ht="28.5">
       <c r="A15" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C15" s="12"/>
       <c r="D15" s="12"/>
       <c r="E15" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H15" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:8" s="6" customFormat="1" ht="28.5">
       <c r="A16" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C16" s="12"/>
       <c r="D16" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E16" s="12"/>
       <c r="F16" s="12"/>
       <c r="G16" s="12"/>
       <c r="H16" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:8" s="3" customFormat="1" ht="28.5">
       <c r="A17" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C17" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17" s="9" t="s">
         <v>28</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>29</v>
       </c>
       <c r="E17" s="9"/>
       <c r="F17" s="9"/>
       <c r="G17" s="9"/>
       <c r="H17" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:8" s="4" customFormat="1" ht="42.75">
       <c r="A18" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
       <c r="H18" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:8" s="4" customFormat="1" ht="28.5">
       <c r="A19" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D19" s="10"/>
       <c r="E19" s="10"/>
       <c r="F19" s="10"/>
       <c r="G19" s="10"/>
       <c r="H19" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:8" s="1" customFormat="1" ht="42.75">
       <c r="A20" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C20" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="D20" s="8" t="s">
-        <v>39</v>
-      </c>
       <c r="E20" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F20" s="8"/>
       <c r="G20" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H20" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:8" s="1" customFormat="1" ht="28.5">
       <c r="A21" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
@@ -1263,18 +1259,18 @@
       <c r="F21" s="8"/>
       <c r="G21" s="8"/>
       <c r="H21" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:8" s="6" customFormat="1" ht="42.75">
       <c r="A22" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D22" s="12"/>
       <c r="E22" s="12"/>
@@ -1284,13 +1280,13 @@
     </row>
     <row r="23" spans="1:8" s="7" customFormat="1" ht="42.75">
       <c r="A23" s="13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D23" s="13"/>
       <c r="E23" s="13"/>
@@ -1300,13 +1296,13 @@
     </row>
     <row r="24" spans="1:8" s="4" customFormat="1" ht="57">
       <c r="A24" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D24" s="10"/>
       <c r="E24" s="10"/>

</xml_diff>